<commit_message>
update with new 2024 data december
</commit_message>
<xml_diff>
--- a/Version_on_pcloud/Data/Data_KS20-527/Compiled_data/K20_averaged.xlsx
+++ b/Version_on_pcloud/Data/Data_KS20-527/Compiled_data/K20_averaged.xlsx
@@ -1645,31 +1645,31 @@
         </is>
       </c>
       <c r="CZ2" t="n">
-        <v>0.004322740231764206</v>
+        <v>0.004121571094013995</v>
       </c>
       <c r="DA2" t="n">
-        <v>0.0003297856184596849</v>
+        <v>0.0003144382496725302</v>
       </c>
       <c r="DB2" t="n">
-        <v>0.0003582743221582286</v>
+        <v>0.0003416011628651941</v>
       </c>
       <c r="DC2" t="n">
-        <v>1.104310113275306e-06</v>
+        <v>1.052918379933622e-06</v>
       </c>
       <c r="DD2" t="n">
-        <v>0.008459892759128965</v>
+        <v>0.008066191254859696</v>
       </c>
       <c r="DE2" t="n">
-        <v>0.0006883329014403164</v>
+        <v>0.0006562996704702154</v>
       </c>
       <c r="DF2" t="n">
-        <v>3.247018350700376e-06</v>
+        <v>3.095910523986615e-06</v>
       </c>
       <c r="DG2" t="n">
-        <v>0.0006962835601127231</v>
+        <v>0.0006638803260742153</v>
       </c>
       <c r="DH2" t="n">
-        <v>0.01261744823646994</v>
+        <v>0.01203026486521681</v>
       </c>
       <c r="DI2" t="n">
         <v>0</v>
@@ -1683,85 +1683,85 @@
       <c r="DL2" t="inlineStr"/>
       <c r="DM2" t="inlineStr"/>
       <c r="DN2" t="n">
-        <v>0.0033521491169325</v>
+        <v>0.003196148776567774</v>
       </c>
       <c r="DO2" t="n">
-        <v>0.000146401791582405</v>
+        <v>0.0001395886312723529</v>
       </c>
       <c r="DP2" t="n">
-        <v>0.004322740231764206</v>
+        <v>0.004121571094013995</v>
       </c>
       <c r="DQ2" t="n">
-        <v>0.0003297856184596849</v>
+        <v>0.0003144382496725302</v>
       </c>
       <c r="DR2" t="n">
-        <v>0.003836849576855474</v>
+        <v>0.003658292532094398</v>
       </c>
       <c r="DS2" t="n">
-        <v>0.0002873723810702059</v>
+        <v>0.0002739988145328696</v>
       </c>
       <c r="DT2" t="n">
-        <v>0.008506966738086185</v>
+        <v>0.008111074532716082</v>
       </c>
       <c r="DU2" t="n">
-        <v>0.0006962835601127231</v>
+        <v>0.0006638803260742153</v>
       </c>
       <c r="DV2" t="n">
-        <v>0.01659841706319401</v>
+        <v>0.01582596971053386</v>
       </c>
       <c r="DW2" t="n">
-        <v>0.0007958935164339218</v>
+        <v>0.0007588546929428664</v>
       </c>
       <c r="DX2" t="n">
-        <v>10.76281389891828</v>
+        <v>10.26194040763103</v>
       </c>
       <c r="DY2" t="n">
-        <v>0.01659841706319401</v>
+        <v>0.01582596971053386</v>
       </c>
       <c r="DZ2" t="n">
-        <v>39.09614776600211</v>
+        <v>37.27671427850061</v>
       </c>
       <c r="EA2" t="n">
-        <v>0.02132793824992076</v>
+        <v>0.02033539122703944</v>
       </c>
       <c r="EB2" t="n">
-        <v>0.3918363953916217</v>
+        <v>0.3736013441107552</v>
       </c>
       <c r="EC2" t="n">
-        <v>0.02773771777896924</v>
+        <v>0.02644687621329951</v>
       </c>
       <c r="ED2" t="n">
-        <v>0.04265587649984189</v>
+        <v>0.0406707824540792</v>
       </c>
       <c r="EE2" t="n">
-        <v>0.008325444746586376</v>
+        <v>0.007938000104536963</v>
       </c>
       <c r="EF2" t="n">
-        <v>0.0001470634639731118</v>
+        <v>0.0001402195111432296</v>
       </c>
       <c r="EG2" t="n">
-        <v>25.2656130986986</v>
+        <v>24.0898168839625</v>
       </c>
       <c r="EH2" t="n">
-        <v>0.008325444746586376</v>
+        <v>0.007938000104536963</v>
       </c>
       <c r="EI2" t="n">
-        <v>63.05776985141785</v>
+        <v>60.12322451458549</v>
       </c>
       <c r="EJ2" t="n">
-        <v>0.002896641055696752</v>
+        <v>0.002761838881079758</v>
       </c>
       <c r="EK2" t="n">
         <v>0</v>
       </c>
       <c r="EL2" t="n">
-        <v>0.1051753663497599</v>
+        <v>0.1002807771246959</v>
       </c>
       <c r="EM2" t="n">
-        <v>0.02317357435362247</v>
+        <v>0.02209513620528016</v>
       </c>
       <c r="EN2" t="n">
-        <v>0.005793282111393329</v>
+        <v>0.005523677762159264</v>
       </c>
       <c r="EO2" t="inlineStr"/>
       <c r="EP2" t="inlineStr"/>
@@ -1779,28 +1779,28 @@
       <c r="FB2" t="inlineStr"/>
       <c r="FC2" t="inlineStr"/>
       <c r="FD2" t="n">
-        <v>0.114260511913241</v>
+        <v>0.1089431235373258</v>
       </c>
       <c r="FE2" t="n">
-        <v>0.08761851201110904</v>
+        <v>0.08354097332795805</v>
       </c>
       <c r="FF2" t="n">
-        <v>0.2313875424123038</v>
+        <v>0.2206193653076095</v>
       </c>
       <c r="FG2" t="n">
-        <v>0.0001343784298858622</v>
+        <v>0.0001281248056977315</v>
       </c>
       <c r="FH2" t="n">
-        <v>0.02377658922874368</v>
+        <v>0.02267008832946689</v>
       </c>
       <c r="FI2" t="n">
-        <v>0.03780884789117619</v>
+        <v>0.03604932200671356</v>
       </c>
       <c r="FJ2" t="n">
-        <v>0.03834466936431745</v>
+        <v>0.03656020773586825</v>
       </c>
       <c r="FK2" t="n">
-        <v>0.0001326314244389507</v>
+        <v>0.0001264591013608934</v>
       </c>
       <c r="FL2" t="n">
         <v>0</v>
@@ -1809,13 +1809,13 @@
         <v>0</v>
       </c>
       <c r="FN2" t="n">
-        <v>1.032795558988644</v>
+        <v>0.9847319278346619</v>
       </c>
       <c r="FO2" t="n">
         <v>0</v>
       </c>
       <c r="FP2" t="n">
-        <v>334.3606834941355</v>
+        <v>318.8004030262446</v>
       </c>
       <c r="FQ2" t="inlineStr"/>
       <c r="FR2" t="inlineStr"/>
@@ -1823,16 +1823,16 @@
       <c r="FT2" t="inlineStr"/>
       <c r="FU2" t="inlineStr"/>
       <c r="FV2" t="n">
-        <v>334.3606834941355</v>
+        <v>318.8004030262446</v>
       </c>
       <c r="FW2" t="n">
-        <v>2.730013713174719e-07</v>
+        <v>2.602965943640123e-07</v>
       </c>
       <c r="FX2" t="n">
-        <v>3.028812817299493e-07</v>
+        <v>2.887859710303373e-07</v>
       </c>
       <c r="FY2" t="n">
-        <v>2.431219990892047e-07</v>
+        <v>2.318077307103913e-07</v>
       </c>
       <c r="FZ2" t="inlineStr">
         <is>
@@ -2153,31 +2153,31 @@
         </is>
       </c>
       <c r="CZ3" t="n">
-        <v>0.00408838938787506</v>
+        <v>0.003898126331607524</v>
       </c>
       <c r="DA3" t="n">
-        <v>0.0005702007352693688</v>
+        <v>0.0005436650694396729</v>
       </c>
       <c r="DB3" t="n">
-        <v>0.0007344163297545911</v>
+        <v>0.0007002384953520575</v>
       </c>
       <c r="DC3" t="n">
-        <v>1.021336776750768e-06</v>
+        <v>9.738064076524554e-07</v>
       </c>
       <c r="DD3" t="n">
-        <v>0.008039157794246059</v>
+        <v>0.007665036205855074</v>
       </c>
       <c r="DE3" t="n">
-        <v>0.001446597876742848</v>
+        <v>0.001379276957156411</v>
       </c>
       <c r="DF3" t="n">
-        <v>4.160558259896129e-06</v>
+        <v>3.966936651187698e-06</v>
       </c>
       <c r="DG3" t="n">
-        <v>0.001512726978834147</v>
+        <v>0.001442328582060869</v>
       </c>
       <c r="DH3" t="n">
-        <v>0.009465727652959553</v>
+        <v>0.009025217197084384</v>
       </c>
       <c r="DI3" t="n">
         <v>0</v>
@@ -2191,85 +2191,85 @@
       <c r="DL3" t="inlineStr"/>
       <c r="DM3" t="inlineStr"/>
       <c r="DN3" t="n">
-        <v>0.003185437034258311</v>
+        <v>0.00303719504256277</v>
       </c>
       <c r="DO3" t="n">
-        <v>0.0001457505099162974</v>
+        <v>0.0001389676585686582</v>
       </c>
       <c r="DP3" t="n">
-        <v>0.00408838938787506</v>
+        <v>0.003898126331607524</v>
       </c>
       <c r="DQ3" t="n">
-        <v>0.0005702007352693688</v>
+        <v>0.0005436650694396729</v>
       </c>
       <c r="DR3" t="n">
-        <v>0.003677673528328275</v>
+        <v>0.003506524124719863</v>
       </c>
       <c r="DS3" t="n">
-        <v>0.0005663805311062444</v>
+        <v>0.0005400226476868536</v>
       </c>
       <c r="DT3" t="n">
-        <v>0.008059693219737435</v>
+        <v>0.007684615965818736</v>
       </c>
       <c r="DU3" t="n">
-        <v>0.001512726978834148</v>
+        <v>0.001442328582060869</v>
       </c>
       <c r="DV3" t="n">
-        <v>0.01013416766046411</v>
+        <v>0.009662549737418471</v>
       </c>
       <c r="DW3" t="n">
-        <v>0.001669571262579826</v>
+        <v>0.001591873738949394</v>
       </c>
       <c r="DX3" t="n">
-        <v>8.319207744056161</v>
+        <v>7.932053356119781</v>
       </c>
       <c r="DY3" t="n">
-        <v>0.0101243186814978</v>
+        <v>0.009653159104427272</v>
       </c>
       <c r="DZ3" t="n">
-        <v>32.13935363252602</v>
+        <v>30.64367133114799</v>
       </c>
       <c r="EA3" t="n">
-        <v>0.01936516374653651</v>
+        <v>0.01846395916693758</v>
       </c>
       <c r="EB3" t="n">
-        <v>1.242663918801037</v>
+        <v>1.184833557582112</v>
       </c>
       <c r="EC3" t="n">
-        <v>0.01564004867616614</v>
+        <v>0.01491220130670441</v>
       </c>
       <c r="ED3" t="n">
-        <v>0.03873032749307292</v>
+        <v>0.03692791833387508</v>
       </c>
       <c r="EE3" t="n">
-        <v>0.002123097192580595</v>
+        <v>0.002024293746508091</v>
       </c>
       <c r="EF3" t="n">
-        <v>1.971772198250471e-05</v>
+        <v>1.880011025546369e-05</v>
       </c>
       <c r="EG3" t="n">
-        <v>8.448103902719586</v>
+        <v>8.054951021302871</v>
       </c>
       <c r="EH3" t="n">
-        <v>0.002123097192580595</v>
+        <v>0.002024293746493335</v>
       </c>
       <c r="EI3" t="n">
-        <v>21.40122705014635</v>
+        <v>20.40526935626539</v>
       </c>
       <c r="EJ3" t="n">
-        <v>0.002397154833449374</v>
+        <v>0.002285597454323184</v>
       </c>
       <c r="EK3" t="n">
         <v>0</v>
       </c>
       <c r="EL3" t="n">
-        <v>0.1054926105635422</v>
+        <v>0.1005832576141919</v>
       </c>
       <c r="EM3" t="n">
-        <v>0.004487554211106231</v>
+        <v>0.0042787150575013</v>
       </c>
       <c r="EN3" t="n">
-        <v>0.004794309666898501</v>
+        <v>0.00457119490864614</v>
       </c>
       <c r="EO3" t="n">
         <v>0</v>
@@ -2281,13 +2281,13 @@
         <v>0</v>
       </c>
       <c r="ER3" t="n">
-        <v>0.05410244670927221</v>
+        <v>0.0515846589239724</v>
       </c>
       <c r="ES3" t="n">
-        <v>5.812898821264435</v>
+        <v>5.542381561145443</v>
       </c>
       <c r="ET3" t="n">
-        <v>0.0242853883655151</v>
+        <v>0.02315520927181866</v>
       </c>
       <c r="EU3" t="inlineStr"/>
       <c r="EV3" t="inlineStr"/>
@@ -2299,28 +2299,28 @@
       <c r="FB3" t="inlineStr"/>
       <c r="FC3" t="inlineStr"/>
       <c r="FD3" t="n">
-        <v>0.01651155250837109</v>
+        <v>0.01574314760709608</v>
       </c>
       <c r="FE3" t="n">
-        <v>0.01366950033002337</v>
+        <v>0.01303335717835754</v>
       </c>
       <c r="FF3" t="n">
-        <v>0.03140102735651599</v>
+        <v>0.02993970484831542</v>
       </c>
       <c r="FG3" t="n">
-        <v>6.936164809210311e-05</v>
+        <v>6.613373658423826e-05</v>
       </c>
       <c r="FH3" t="n">
-        <v>0.005875630067743543</v>
+        <v>0.005602193457839931</v>
       </c>
       <c r="FI3" t="n">
-        <v>0.00845092686027692</v>
+        <v>0.008057642605724875</v>
       </c>
       <c r="FJ3" t="n">
-        <v>0.009720235566178903</v>
+        <v>0.009267880971006033</v>
       </c>
       <c r="FK3" t="n">
-        <v>5.000022869217896e-06</v>
+        <v>4.767334751171718e-06</v>
       </c>
       <c r="FL3" t="n">
         <v>0</v>
@@ -2335,7 +2335,7 @@
         <v>0</v>
       </c>
       <c r="FP3" t="n">
-        <v>243.0676174784827</v>
+        <v>231.7558799227948</v>
       </c>
       <c r="FQ3" t="inlineStr"/>
       <c r="FR3" t="inlineStr"/>
@@ -2343,16 +2343,16 @@
       <c r="FT3" t="inlineStr"/>
       <c r="FU3" t="inlineStr"/>
       <c r="FV3" t="n">
-        <v>243.0676174784827</v>
+        <v>231.7558799227948</v>
       </c>
       <c r="FW3" t="n">
-        <v>1.984617096869084e-07</v>
+        <v>1.892258155404329e-07</v>
       </c>
       <c r="FX3" t="n">
-        <v>1.585202181541789e-07</v>
+        <v>1.511430976542597e-07</v>
       </c>
       <c r="FY3" t="n">
-        <v>2.384033529819596e-07</v>
+        <v>2.273086782885878e-07</v>
       </c>
       <c r="FZ3" t="inlineStr">
         <is>
@@ -2679,31 +2679,31 @@
         </is>
       </c>
       <c r="CZ4" t="n">
-        <v>0.009054495142913278</v>
+        <v>0.008633122383273701</v>
       </c>
       <c r="DA4" t="n">
-        <v>5.64000887777935e-05</v>
+        <v>5.377537467975624e-05</v>
       </c>
       <c r="DB4" t="n">
-        <v>8.938435664518827e-05</v>
+        <v>8.522464012497288e-05</v>
       </c>
       <c r="DC4" t="n">
-        <v>2.27136892272914e-06</v>
+        <v>2.165665294197172e-06</v>
       </c>
       <c r="DD4" t="n">
-        <v>0.01778869880132437</v>
+        <v>0.01696085881841999</v>
       </c>
       <c r="DE4" t="n">
-        <v>0.0001787869684447992</v>
+        <v>0.0001704666858567483</v>
       </c>
       <c r="DF4" t="n">
-        <v>2.910410981912523e-06</v>
+        <v>2.774967990583252e-06</v>
       </c>
       <c r="DG4" t="n">
-        <v>0.0001941882761955295</v>
+        <v>0.0001851512566225278</v>
       </c>
       <c r="DH4" t="n">
-        <v>0.01889620773241733</v>
+        <v>0.01801682715147323</v>
       </c>
       <c r="DI4" t="n">
         <v>0</v>
@@ -2717,112 +2717,112 @@
       <c r="DL4" t="inlineStr"/>
       <c r="DM4" t="inlineStr"/>
       <c r="DN4" t="n">
-        <v>0.007048596557413545</v>
+        <v>0.006720573124179088</v>
       </c>
       <c r="DO4" t="n">
-        <v>8.418041988961664e-05</v>
+        <v>8.026288111173488e-05</v>
       </c>
       <c r="DP4" t="n">
-        <v>0.009054495142913278</v>
+        <v>0.008633122383273701</v>
       </c>
       <c r="DQ4" t="n">
-        <v>5.64000887777935e-05</v>
+        <v>5.377537467975624e-05</v>
       </c>
       <c r="DR4" t="n">
-        <v>0.008124973388260414</v>
+        <v>0.007746858164322312</v>
       </c>
       <c r="DS4" t="n">
-        <v>6.405609597888887e-05</v>
+        <v>6.107509112899551e-05</v>
       </c>
       <c r="DT4" t="n">
-        <v>0.01781175434269228</v>
+        <v>0.0169828414145919</v>
       </c>
       <c r="DU4" t="n">
-        <v>0.0001941882761955295</v>
+        <v>0.0001851512566225278</v>
       </c>
       <c r="DV4" t="n">
-        <v>0.02751313410621055</v>
+        <v>0.02623274408308158</v>
       </c>
       <c r="DW4" t="n">
-        <v>0.0001663981894604489</v>
+        <v>0.0001586544485687383</v>
       </c>
       <c r="DX4" t="n">
-        <v>40.53507814004808</v>
+        <v>38.64868055868264</v>
       </c>
       <c r="DY4" t="n">
-        <v>0.02751313410617949</v>
+        <v>0.02623274408299633</v>
       </c>
       <c r="DZ4" t="n">
-        <v>98.42631270533592</v>
+        <v>93.84580696192594</v>
       </c>
       <c r="EA4" t="n">
-        <v>0.01052604021233424</v>
+        <v>0.01003618555535543</v>
       </c>
       <c r="EB4" t="n">
-        <v>0.01688795186707846</v>
+        <v>0.01610203031423975</v>
       </c>
       <c r="EC4" t="n">
-        <v>0.008508300658104198</v>
+        <v>0.008112346375556006</v>
       </c>
       <c r="ED4" t="n">
-        <v>0.02105208042466932</v>
+        <v>0.02007237111071136</v>
       </c>
       <c r="EE4" t="n">
-        <v>0.01019675189691494</v>
+        <v>0.009722221465514234</v>
       </c>
       <c r="EF4" t="n">
-        <v>0.0003170680861963331</v>
+        <v>0.0003023125584319004</v>
       </c>
       <c r="EG4" t="n">
-        <v>84.76339691214795</v>
+        <v>80.81872789310843</v>
       </c>
       <c r="EH4" t="n">
-        <v>0.01019675189691494</v>
+        <v>0.009722221465514234</v>
       </c>
       <c r="EI4" t="n">
-        <v>182.1460256070647</v>
+        <v>173.6694211961059</v>
       </c>
       <c r="EJ4" t="n">
-        <v>0.005975936258591885</v>
+        <v>0.005697831658283635</v>
       </c>
       <c r="EK4" t="n">
         <v>0</v>
       </c>
       <c r="EL4" t="n">
-        <v>0.3323365318891037</v>
+        <v>0.3168704501958851</v>
       </c>
       <c r="EM4" t="n">
-        <v>0.006505488333767475</v>
+        <v>0.006202739751020928</v>
       </c>
       <c r="EN4" t="n">
-        <v>0.01195187251718377</v>
+        <v>0.01139566331656727</v>
       </c>
       <c r="EO4" t="n">
-        <v>0.07306327093926594</v>
+        <v>0.06966309548848572</v>
       </c>
       <c r="EP4" t="n">
-        <v>22.02546687588954</v>
+        <v>21.00045867682866</v>
       </c>
       <c r="EQ4" t="n">
-        <v>0.03195505007803161</v>
+        <v>0.03046794478687258</v>
       </c>
       <c r="ER4" t="n">
-        <v>0.03424317433583759</v>
+        <v>0.03264958566623857</v>
       </c>
       <c r="ES4" t="n">
-        <v>22.14390119421583</v>
+        <v>21.11338136863559</v>
       </c>
       <c r="ET4" t="n">
-        <v>0.09426712321316512</v>
+        <v>0.08988017537955771</v>
       </c>
       <c r="EU4" t="n">
-        <v>0.01746713185831379</v>
+        <v>0.01617142175980815</v>
       </c>
       <c r="EV4" t="n">
-        <v>4.547693527886992</v>
+        <v>4.210346075723318</v>
       </c>
       <c r="EW4" t="n">
-        <v>0.0034120021555427</v>
+        <v>0.003158900176068705</v>
       </c>
       <c r="EX4" t="inlineStr"/>
       <c r="EY4" t="inlineStr"/>
@@ -2831,28 +2831,28 @@
       <c r="FB4" t="inlineStr"/>
       <c r="FC4" t="inlineStr"/>
       <c r="FD4" t="n">
-        <v>0.02444657925049204</v>
+        <v>0.02330889875037172</v>
       </c>
       <c r="FE4" t="n">
-        <v>0.01562506352471102</v>
+        <v>0.01489791352539781</v>
       </c>
       <c r="FF4" t="n">
-        <v>0.04944916588469294</v>
+        <v>0.04714792974045415</v>
       </c>
       <c r="FG4" t="n">
-        <v>0.0001392567895916149</v>
+        <v>0.0001327761391740501</v>
       </c>
       <c r="FH4" t="n">
-        <v>0.0161178301658752</v>
+        <v>0.01536774808297608</v>
       </c>
       <c r="FI4" t="n">
-        <v>0.02370618238149936</v>
+        <v>0.02260295803459265</v>
       </c>
       <c r="FJ4" t="n">
-        <v>0.02561898241138573</v>
+        <v>0.02442674130379713</v>
       </c>
       <c r="FK4" t="n">
-        <v>5.306897909925677e-05</v>
+        <v>5.059928622059757e-05</v>
       </c>
       <c r="FL4" t="n">
         <v>0</v>
@@ -2867,7 +2867,7 @@
         <v>0</v>
       </c>
       <c r="FP4" t="n">
-        <v>282.2594551117811</v>
+        <v>269.1238309099282</v>
       </c>
       <c r="FQ4" t="inlineStr"/>
       <c r="FR4" t="inlineStr"/>
@@ -2875,16 +2875,16 @@
       <c r="FT4" t="inlineStr"/>
       <c r="FU4" t="inlineStr"/>
       <c r="FV4" t="n">
-        <v>282.2594551117811</v>
+        <v>269.1238309099282</v>
       </c>
       <c r="FW4" t="n">
-        <v>2.304613613661031e-07</v>
+        <v>2.197362863264472e-07</v>
       </c>
       <c r="FX4" t="n">
-        <v>2.599200772177675e-07</v>
+        <v>2.478240697835068e-07</v>
       </c>
       <c r="FY4" t="n">
-        <v>2.010029623491028e-07</v>
+        <v>1.916488049760567e-07</v>
       </c>
       <c r="FZ4" t="inlineStr">
         <is>
@@ -3199,31 +3199,31 @@
         </is>
       </c>
       <c r="CZ5" t="n">
-        <v>0.009044423364923568</v>
+        <v>0.008623519319753378</v>
       </c>
       <c r="DA5" t="n">
-        <v>0.001057922099540897</v>
+        <v>0.001008689144248397</v>
       </c>
       <c r="DB5" t="n">
-        <v>0.001182862803358922</v>
+        <v>0.001127815431212898</v>
       </c>
       <c r="DC5" t="n">
-        <v>2.28415963615858e-06</v>
+        <v>2.177860760942002e-06</v>
       </c>
       <c r="DD5" t="n">
-        <v>0.01774382658212686</v>
+        <v>0.01691807483611963</v>
       </c>
       <c r="DE5" t="n">
-        <v>0.002364240749587454</v>
+        <v>0.002254215106701593</v>
       </c>
       <c r="DF5" t="n">
-        <v>4.337462670620385e-06</v>
+        <v>4.135608388685828e-06</v>
       </c>
       <c r="DG5" t="n">
-        <v>0.002376618284228738</v>
+        <v>0.00226601662292915</v>
       </c>
       <c r="DH5" t="n">
-        <v>0.008197560612767394</v>
+        <v>0.007816067367347333</v>
       </c>
       <c r="DI5" t="n">
         <v>0</v>
@@ -3237,97 +3237,97 @@
       <c r="DL5" t="inlineStr"/>
       <c r="DM5" t="inlineStr"/>
       <c r="DN5" t="n">
-        <v>0.007030816382864745</v>
+        <v>0.00670362039291657</v>
       </c>
       <c r="DO5" t="n">
-        <v>0.0003063169828414956</v>
+        <v>0.0002920617835899507</v>
       </c>
       <c r="DP5" t="n">
-        <v>0.009044423364923568</v>
+        <v>0.008623519319753378</v>
       </c>
       <c r="DQ5" t="n">
-        <v>0.001057922099540897</v>
+        <v>0.001008689144248397</v>
       </c>
       <c r="DR5" t="n">
-        <v>0.008083544418282861</v>
+        <v>0.007707357191337734</v>
       </c>
       <c r="DS5" t="n">
-        <v>0.001042767880579611</v>
+        <v>0.000994240163399574</v>
       </c>
       <c r="DT5" t="n">
-        <v>0.01781144383947725</v>
+        <v>0.01698254536139131</v>
       </c>
       <c r="DU5" t="n">
-        <v>0.002376618284228738</v>
+        <v>0.00226601662292915</v>
       </c>
       <c r="DV5" t="n">
-        <v>0.03903159675256073</v>
+        <v>0.03721516730204787</v>
       </c>
       <c r="DW5" t="n">
-        <v>0.001791766470640966</v>
+        <v>0.001708382298420771</v>
       </c>
       <c r="DX5" t="n">
-        <v>139.3919537699578</v>
+        <v>132.9050131615059</v>
       </c>
       <c r="DY5" t="n">
-        <v>0.03903159675256073</v>
+        <v>0.03721516730204787</v>
       </c>
       <c r="DZ5" t="n">
-        <v>387.2520597673626</v>
+        <v>369.2303515964784</v>
       </c>
       <c r="EA5" t="n">
-        <v>0.007343411282741102</v>
+        <v>0.007001667935537704</v>
       </c>
       <c r="EB5" t="n">
-        <v>0.6258761035799425</v>
+        <v>0.5967494502662745</v>
       </c>
       <c r="EC5" t="n">
-        <v>0.0349691373817835</v>
+        <v>0.03334176427172011</v>
       </c>
       <c r="ED5" t="n">
-        <v>0.01468682256548219</v>
+        <v>0.0140033358710753</v>
       </c>
       <c r="EE5" t="n">
-        <v>0.02171080970215393</v>
+        <v>0.0207004448332303</v>
       </c>
       <c r="EF5" t="n">
-        <v>0.001775024536745319</v>
+        <v>0.001692419490779649</v>
       </c>
       <c r="EG5" t="n">
-        <v>268.9897531756195</v>
+        <v>256.4716665433589</v>
       </c>
       <c r="EH5" t="n">
-        <v>0.02173472249408961</v>
+        <v>0.02072324478573048</v>
       </c>
       <c r="EI5" t="n">
-        <v>623.5008966979599</v>
+        <v>594.4847793625852</v>
       </c>
       <c r="EJ5" t="n">
-        <v>0.003600329773611842</v>
+        <v>0.003432779748085921</v>
       </c>
       <c r="EK5" t="n">
         <v>0</v>
       </c>
       <c r="EL5" t="n">
-        <v>0.1921895364291654</v>
+        <v>0.1832455330296621</v>
       </c>
       <c r="EM5" t="n">
-        <v>0.01465617156491003</v>
+        <v>0.01397411128870678</v>
       </c>
       <c r="EN5" t="n">
-        <v>0.007200659547223514</v>
+        <v>0.006865559496171732</v>
       </c>
       <c r="EO5" t="inlineStr"/>
       <c r="EP5" t="inlineStr"/>
       <c r="EQ5" t="inlineStr"/>
       <c r="ER5" t="n">
-        <v>0.01704398548289757</v>
+        <v>0.01577966434030698</v>
       </c>
       <c r="ES5" t="n">
-        <v>12.94490295100184</v>
+        <v>11.98465134164255</v>
       </c>
       <c r="ET5" t="n">
-        <v>0.04311089749153597</v>
+        <v>0.03991293541689809</v>
       </c>
       <c r="EU5" t="inlineStr"/>
       <c r="EV5" t="inlineStr"/>
@@ -3339,28 +3339,28 @@
       <c r="FB5" t="inlineStr"/>
       <c r="FC5" t="inlineStr"/>
       <c r="FD5" t="n">
-        <v>0.02055140496565893</v>
+        <v>0.01959499579119182</v>
       </c>
       <c r="FE5" t="n">
-        <v>0.02218897859135291</v>
+        <v>0.02115636098042637</v>
       </c>
       <c r="FF5" t="n">
-        <v>0.04005131262213796</v>
+        <v>0.03818742823538833</v>
       </c>
       <c r="FG5" t="n">
-        <v>0.001892312927832682</v>
+        <v>0.001804249583834256</v>
       </c>
       <c r="FH5" t="n">
-        <v>0.009725711643574624</v>
+        <v>0.009273102205938688</v>
       </c>
       <c r="FI5" t="n">
-        <v>0.01607265933104015</v>
+        <v>0.015324679381836</v>
       </c>
       <c r="FJ5" t="n">
-        <v>0.01620590174735493</v>
+        <v>0.0154517210410927</v>
       </c>
       <c r="FK5" t="n">
-        <v>0.0007655127353481321</v>
+        <v>0.0007298877547455057</v>
       </c>
       <c r="FL5" t="n">
         <v>0</v>
@@ -3375,7 +3375,7 @@
         <v>0</v>
       </c>
       <c r="FP5" t="n">
-        <v>229.4730194743298</v>
+        <v>218.7939393099986</v>
       </c>
       <c r="FQ5" t="inlineStr"/>
       <c r="FR5" t="inlineStr"/>
@@ -3383,16 +3383,16 @@
       <c r="FT5" t="inlineStr"/>
       <c r="FU5" t="inlineStr"/>
       <c r="FV5" t="n">
-        <v>229.4730194743298</v>
+        <v>218.7939393099986</v>
       </c>
       <c r="FW5" t="n">
-        <v>3.037042369017686e-07</v>
+        <v>2.895706280777925e-07</v>
       </c>
       <c r="FX5" t="n">
-        <v>3.441583220316917e-07</v>
+        <v>3.281420848418987e-07</v>
       </c>
       <c r="FY5" t="n">
-        <v>2.632504144086165e-07</v>
+        <v>2.509994217293434e-07</v>
       </c>
       <c r="FZ5" t="inlineStr">
         <is>
@@ -3713,31 +3713,31 @@
         </is>
       </c>
       <c r="CZ6" t="n">
-        <v>0.003291579308359979</v>
+        <v>0.00313839773005612</v>
       </c>
       <c r="DA6" t="n">
-        <v>9.124394126250878e-05</v>
+        <v>8.6997684489125e-05</v>
       </c>
       <c r="DB6" t="n">
-        <v>0.0001085894741268126</v>
+        <v>0.000103536001165768</v>
       </c>
       <c r="DC6" t="n">
-        <v>8.364052708717801e-07</v>
+        <v>7.974811352240221e-07</v>
       </c>
       <c r="DD6" t="n">
-        <v>0.006449237862841694</v>
+        <v>0.006149107031357073</v>
       </c>
       <c r="DE6" t="n">
-        <v>0.0002061521219527994</v>
+        <v>0.0001965583359755892</v>
       </c>
       <c r="DF6" t="n">
-        <v>2.594067245425164e-06</v>
+        <v>2.473346072500333e-06</v>
       </c>
       <c r="DG6" t="n">
-        <v>0.0002076951583747043</v>
+        <v>0.000198029563477719</v>
       </c>
       <c r="DH6" t="n">
-        <v>0.04135053405539882</v>
+        <v>0.03942618726714858</v>
       </c>
       <c r="DI6" t="n">
         <v>0</v>
@@ -3751,136 +3751,136 @@
       <c r="DL6" t="inlineStr"/>
       <c r="DM6" t="inlineStr"/>
       <c r="DN6" t="n">
-        <v>0.002555446933220615</v>
+        <v>0.002436523049628237</v>
       </c>
       <c r="DO6" t="n">
-        <v>4.937443287872614e-05</v>
+        <v>4.707667461508285e-05</v>
       </c>
       <c r="DP6" t="n">
-        <v>0.003291579308359979</v>
+        <v>0.00313839773005612</v>
       </c>
       <c r="DQ6" t="n">
-        <v>9.124394126250878e-05</v>
+        <v>8.6997684489125e-05</v>
       </c>
       <c r="DR6" t="n">
-        <v>0.002931093356624508</v>
+        <v>0.00279468786112772</v>
       </c>
       <c r="DS6" t="n">
-        <v>7.950413913300193e-05</v>
+        <v>7.580422235349371e-05</v>
       </c>
       <c r="DT6" t="n">
-        <v>0.006486780098300546</v>
+        <v>0.006184902148396849</v>
       </c>
       <c r="DU6" t="n">
-        <v>0.0002076951583747036</v>
+        <v>0.0001980295634777183</v>
       </c>
       <c r="DV6" t="n">
-        <v>0.01622292395150941</v>
+        <v>0.01546795107595128</v>
       </c>
       <c r="DW6" t="n">
-        <v>0.0002430602641854932</v>
+        <v>0.0002317488688330182</v>
       </c>
       <c r="DX6" t="n">
-        <v>37.55968612036185</v>
+        <v>35.81175557957203</v>
       </c>
       <c r="DY6" t="n">
-        <v>0.01622292395150941</v>
+        <v>0.01546795107595128</v>
       </c>
       <c r="DZ6" t="n">
-        <v>115.4225644244481</v>
+        <v>110.0510971335006</v>
       </c>
       <c r="EA6" t="n">
-        <v>0.009597899465110334</v>
+        <v>0.009151238075322976</v>
       </c>
       <c r="EB6" t="n">
-        <v>0.3946198986123727</v>
+        <v>0.3762553102987861</v>
       </c>
       <c r="EC6" t="n">
-        <v>0.02096835261179956</v>
+        <v>0.01999253977346099</v>
       </c>
       <c r="ED6" t="n">
-        <v>0.01919579893022058</v>
+        <v>0.01830247615064589</v>
       </c>
       <c r="EE6" t="n">
-        <v>0.00981898611549463</v>
+        <v>0.009362035925299618</v>
       </c>
       <c r="EF6" t="n">
-        <v>0.0001473998902282967</v>
+        <v>0.0001405402809915878</v>
       </c>
       <c r="EG6" t="n">
-        <v>88.87835736950412</v>
+        <v>84.74218874542244</v>
       </c>
       <c r="EH6" t="n">
-        <v>0.0098189861154886</v>
+        <v>0.009362035925428435</v>
       </c>
       <c r="EI6" t="n">
-        <v>213.5030070997927</v>
+        <v>203.5671299610883</v>
       </c>
       <c r="EJ6" t="n">
-        <v>0.00540140326880223</v>
+        <v>0.005150035946231741</v>
       </c>
       <c r="EK6" t="n">
         <v>0</v>
       </c>
       <c r="EL6" t="n">
-        <v>0.06558833343933101</v>
+        <v>0.06253602222536761</v>
       </c>
       <c r="EM6" t="n">
-        <v>0.008525748731123788</v>
+        <v>0.008128982460434661</v>
       </c>
       <c r="EN6" t="n">
-        <v>0.01080280653760447</v>
+        <v>0.01030007189246353</v>
       </c>
       <c r="EO6" t="inlineStr"/>
       <c r="EP6" t="inlineStr"/>
       <c r="EQ6" t="inlineStr"/>
       <c r="ER6" t="n">
-        <v>0.004653989545918983</v>
+        <v>0.004437404922780453</v>
       </c>
       <c r="ES6" t="n">
-        <v>9.818131572462026</v>
+        <v>9.361221150633545</v>
       </c>
       <c r="ET6" t="n">
-        <v>0.138927591374551</v>
+        <v>0.132462260989633</v>
       </c>
       <c r="EU6" t="inlineStr"/>
       <c r="EV6" t="inlineStr"/>
       <c r="EW6" t="inlineStr"/>
       <c r="EX6" t="n">
-        <v>1.77432908235907</v>
+        <v>1.691756401039812</v>
       </c>
       <c r="EY6" t="n">
-        <v>37.73550914092818</v>
+        <v>35.9793962520101</v>
       </c>
       <c r="EZ6" t="n">
-        <v>1.683360111440281</v>
+        <v>1.605020890486599</v>
       </c>
       <c r="FA6" t="inlineStr"/>
       <c r="FB6" t="inlineStr"/>
       <c r="FC6" t="inlineStr"/>
       <c r="FD6" t="n">
-        <v>0.02987128846003352</v>
+        <v>0.02848115603920553</v>
       </c>
       <c r="FE6" t="n">
-        <v>0.01247318828176978</v>
+        <v>0.01189271839528398</v>
       </c>
       <c r="FF6" t="n">
-        <v>0.06037816402618483</v>
+        <v>0.05756832060630127</v>
       </c>
       <c r="FG6" t="n">
-        <v>0.0001918767668734308</v>
+        <v>0.0001829473189592143</v>
       </c>
       <c r="FH6" t="n">
-        <v>0.001898039965519295</v>
+        <v>0.001809710100015624</v>
       </c>
       <c r="FI6" t="n">
-        <v>0.02019194262597058</v>
+        <v>0.01925226189805627</v>
       </c>
       <c r="FJ6" t="n">
-        <v>0.003587816287807302</v>
+        <v>0.003420848607510259</v>
       </c>
       <c r="FK6" t="n">
-        <v>0.0001007317459411725</v>
+        <v>9.604395130429959e-05</v>
       </c>
       <c r="FL6" t="n">
         <v>0</v>
@@ -3895,7 +3895,7 @@
         <v>0</v>
       </c>
       <c r="FP6" t="n">
-        <v>272.007843024178</v>
+        <v>259.3493023049413</v>
       </c>
       <c r="FQ6" t="inlineStr"/>
       <c r="FR6" t="inlineStr"/>
@@ -3903,16 +3903,16 @@
       <c r="FT6" t="inlineStr"/>
       <c r="FU6" t="inlineStr"/>
       <c r="FV6" t="n">
-        <v>272.007843024178</v>
+        <v>259.3493023049413</v>
       </c>
       <c r="FW6" t="n">
-        <v>3.59998463417514e-07</v>
+        <v>3.432450670697337e-07</v>
       </c>
       <c r="FX6" t="n">
-        <v>3.349643949710072e-07</v>
+        <v>3.193760193205641e-07</v>
       </c>
       <c r="FY6" t="n">
-        <v>3.850331941549521e-07</v>
+        <v>3.671147461962039e-07</v>
       </c>
       <c r="FZ6" t="inlineStr">
         <is>
@@ -5919,31 +5919,31 @@
         </is>
       </c>
       <c r="CZ10" t="n">
-        <v>0.003180353479746914</v>
+        <v>0.002944435175931269</v>
       </c>
       <c r="DA10" t="n">
-        <v>0.0002299138208525451</v>
+        <v>0.000212858836560792</v>
       </c>
       <c r="DB10" t="n">
-        <v>0.0002949875659693795</v>
+        <v>0.000273105417757433</v>
       </c>
       <c r="DC10" t="n">
-        <v>2.863224548910697e-06</v>
+        <v>2.650830837543942e-06</v>
       </c>
       <c r="DD10" t="n">
-        <v>0.008026328315454341</v>
+        <v>0.007430936081823092</v>
       </c>
       <c r="DE10" t="n">
-        <v>0.0007444666350819695</v>
+        <v>0.0006892421743689242</v>
       </c>
       <c r="DF10" t="n">
-        <v>4.877823619908153e-07</v>
+        <v>4.515987150456344e-07</v>
       </c>
       <c r="DG10" t="n">
-        <v>0.0007514537494105019</v>
+        <v>0.0006957109852536883</v>
       </c>
       <c r="DH10" t="n">
-        <v>0.001154700538378868</v>
+        <v>0.001069044967649705</v>
       </c>
       <c r="DI10" t="n">
         <v>0</v>
@@ -5957,85 +5957,85 @@
       <c r="DL10" t="inlineStr"/>
       <c r="DM10" t="inlineStr"/>
       <c r="DN10" t="n">
-        <v>0.003180353479746914</v>
+        <v>0.002944435175931269</v>
       </c>
       <c r="DO10" t="n">
-        <v>0.0002299138208525451</v>
+        <v>0.000212858836560792</v>
       </c>
       <c r="DP10" t="n">
-        <v>0.003175544770843698</v>
+        <v>0.002939983176574723</v>
       </c>
       <c r="DQ10" t="n">
-        <v>0.0002659294263441879</v>
+        <v>0.0002462028080304334</v>
       </c>
       <c r="DR10" t="n">
-        <v>0.006061055121614061</v>
+        <v>0.005611446657419663</v>
       </c>
       <c r="DS10" t="n">
-        <v>0.0005289146263253791</v>
+        <v>0.0004896797921157245</v>
       </c>
       <c r="DT10" t="n">
-        <v>0.008056794970347347</v>
+        <v>0.007459142723293881</v>
       </c>
       <c r="DU10" t="n">
-        <v>0.0007514537494105019</v>
+        <v>0.0006957109852536883</v>
       </c>
       <c r="DV10" t="n">
-        <v>0.008700248849600006</v>
+        <v>0.008054865258021768</v>
       </c>
       <c r="DW10" t="n">
-        <v>0.0007643739588897304</v>
+        <v>0.0007076727748828312</v>
       </c>
       <c r="DX10" t="n">
-        <v>10.28552419605363</v>
+        <v>9.522545037403352</v>
       </c>
       <c r="DY10" t="n">
-        <v>0.008700248849600006</v>
+        <v>0.008054865258021768</v>
       </c>
       <c r="DZ10" t="n">
-        <v>15.19746728289651</v>
+        <v>14.07012067614134</v>
       </c>
       <c r="EA10" t="n">
-        <v>0.02095589240727456</v>
+        <v>0.0194013863993258</v>
       </c>
       <c r="EB10" t="n">
-        <v>0.1308909930984163</v>
+        <v>0.121181512289704</v>
       </c>
       <c r="EC10" t="n">
-        <v>0.1209309067489354</v>
+        <v>0.1119602641518845</v>
       </c>
       <c r="ED10" t="n">
-        <v>0.04191178481454912</v>
+        <v>0.0388027727986516</v>
       </c>
       <c r="EE10" t="n">
-        <v>0.0006434538792512908</v>
+        <v>0.0005957225347026574</v>
       </c>
       <c r="EF10" t="n">
-        <v>0.0001876343740133369</v>
+        <v>0.0001737156748697879</v>
       </c>
       <c r="EG10" t="n">
-        <v>11.88677231716533</v>
+        <v>11.00501273265161</v>
       </c>
       <c r="EH10" t="n">
-        <v>0.0006434538792512908</v>
+        <v>0.0005957225347026574</v>
       </c>
       <c r="EI10" t="n">
-        <v>11.99813235493582</v>
+        <v>11.10811209393097</v>
       </c>
       <c r="EJ10" t="n">
-        <v>0.01278010923746028</v>
+        <v>0.01183208200932955</v>
       </c>
       <c r="EK10" t="n">
         <v>0</v>
       </c>
       <c r="EL10" t="n">
-        <v>0.0738874991190267</v>
+        <v>0.06840653180632149</v>
       </c>
       <c r="EM10" t="n">
-        <v>0.0590380458681036</v>
+        <v>0.05465860951598416</v>
       </c>
       <c r="EN10" t="n">
-        <v>0.02556021847492056</v>
+        <v>0.02366416401865911</v>
       </c>
       <c r="EO10" t="inlineStr"/>
       <c r="EP10" t="inlineStr"/>
@@ -6053,28 +6053,28 @@
       <c r="FB10" t="inlineStr"/>
       <c r="FC10" t="inlineStr"/>
       <c r="FD10" t="n">
-        <v>0.04011890585311654</v>
+        <v>0.03714288941969795</v>
       </c>
       <c r="FE10" t="n">
-        <v>0.05247785689348114</v>
+        <v>0.04858505470497238</v>
       </c>
       <c r="FF10" t="n">
-        <v>0.03574080438673548</v>
+        <v>0.03308955508327872</v>
       </c>
       <c r="FG10" t="n">
-        <v>0.0008309445869828848</v>
+        <v>0.0007693052004259556</v>
       </c>
       <c r="FH10" t="n">
-        <v>0.001517988675621087</v>
+        <v>0.001405384427117133</v>
       </c>
       <c r="FI10" t="n">
-        <v>0.02218305298668387</v>
+        <v>0.02053751632939136</v>
       </c>
       <c r="FJ10" t="n">
-        <v>0.005107065445799502</v>
+        <v>0.004728223840575032</v>
       </c>
       <c r="FK10" t="n">
-        <v>0.000283960037427215</v>
+        <v>0.0002628959101822814</v>
       </c>
       <c r="FL10" t="n">
         <v>0</v>
@@ -6089,7 +6089,7 @@
         <v>0</v>
       </c>
       <c r="FP10" t="n">
-        <v>151.8431207968726</v>
+        <v>140.5794132459365</v>
       </c>
       <c r="FQ10" t="n">
         <v>0</v>
@@ -6107,16 +6107,16 @@
         <v>0</v>
       </c>
       <c r="FV10" t="n">
-        <v>151.8431207968726</v>
+        <v>140.5794132459365</v>
       </c>
       <c r="FW10" t="n">
-        <v>1.239780340253055e-07</v>
+        <v>1.147813558907516e-07</v>
       </c>
       <c r="FX10" t="n">
-        <v>1.276013765579303e-07</v>
+        <v>1.181359191710326e-07</v>
       </c>
       <c r="FY10" t="n">
-        <v>1.20354691562121e-07</v>
+        <v>1.114267925569197e-07</v>
       </c>
       <c r="FZ10" t="inlineStr">
         <is>
@@ -19017,31 +19017,31 @@
         </is>
       </c>
       <c r="CZ34" t="n">
-        <v>0.001998452903821577</v>
+        <v>0.001905450080163094</v>
       </c>
       <c r="DA34" t="n">
-        <v>0.0005849213964367269</v>
+        <v>0.0005577006691517093</v>
       </c>
       <c r="DB34" t="n">
-        <v>0.0007694521557218346</v>
+        <v>0.0007336438446951432</v>
       </c>
       <c r="DC34" t="n">
-        <v>3.182227219287229e-06</v>
+        <v>3.03413460406939e-06</v>
       </c>
       <c r="DD34" t="n">
-        <v>0.005043539729509236</v>
+        <v>0.004808826449459376</v>
       </c>
       <c r="DE34" t="n">
-        <v>0.001941883398873558</v>
+        <v>0.001851513173503015</v>
       </c>
       <c r="DF34" t="n">
-        <v>4.513786181963119e-07</v>
+        <v>4.303726260355536e-07</v>
       </c>
       <c r="DG34" t="n">
-        <v>0.001949184824098821</v>
+        <v>0.001858474809303476</v>
       </c>
       <c r="DH34" t="n">
-        <v>0.06748036751530127</v>
+        <v>0.06434000593438227</v>
       </c>
       <c r="DI34" t="n">
         <v>0</v>
@@ -19055,103 +19055,103 @@
       <c r="DL34" t="inlineStr"/>
       <c r="DM34" t="inlineStr"/>
       <c r="DN34" t="n">
-        <v>0.001998452903821577</v>
+        <v>0.001905450080163094</v>
       </c>
       <c r="DO34" t="n">
-        <v>0.0005849213964367269</v>
+        <v>0.0005577006691517093</v>
       </c>
       <c r="DP34" t="n">
-        <v>0.002017906098740378</v>
+        <v>0.001923997973759467</v>
       </c>
       <c r="DQ34" t="n">
-        <v>0.0006865435919034456</v>
+        <v>0.0006545936307662285</v>
       </c>
       <c r="DR34" t="n">
-        <v>0.003676357003963363</v>
+        <v>0.003505268867990076</v>
       </c>
       <c r="DS34" t="n">
-        <v>0.001382520524372114</v>
+        <v>0.00131818159885301</v>
       </c>
       <c r="DT34" t="n">
-        <v>0.005074945668763508</v>
+        <v>0.004838770837617376</v>
       </c>
       <c r="DU34" t="n">
-        <v>0.001949184824098821</v>
+        <v>0.001858474809303476</v>
       </c>
       <c r="DV34" t="n">
-        <v>0.005052701067364646</v>
+        <v>0.004817561442466234</v>
       </c>
       <c r="DW34" t="n">
-        <v>0.001682399330552294</v>
+        <v>0.001604104821853441</v>
       </c>
       <c r="DX34" t="n">
-        <v>34.15758874038944</v>
+        <v>32.56798300279781</v>
       </c>
       <c r="DY34" t="n">
-        <v>0.005052701067186797</v>
+        <v>0.004817561442260395</v>
       </c>
       <c r="DZ34" t="n">
-        <v>43.21661127917424</v>
+        <v>41.20542208866173</v>
       </c>
       <c r="EA34" t="n">
-        <v>0.009997229475394906</v>
+        <v>0.009531984300892376</v>
       </c>
       <c r="EB34" t="n">
-        <v>0.6785034378868143</v>
+        <v>0.6469276446995978</v>
       </c>
       <c r="EC34" t="n">
-        <v>0.0355813134470743</v>
+        <v>0.03392545124800647</v>
       </c>
       <c r="ED34" t="n">
-        <v>0.0199944589507897</v>
+        <v>0.01906396860178466</v>
       </c>
       <c r="EE34" t="n">
-        <v>0.002506061220456465</v>
+        <v>0.002389435620152463</v>
       </c>
       <c r="EF34" t="n">
-        <v>0.004126199724554521</v>
+        <v>0.003934177073118203</v>
       </c>
       <c r="EG34" t="n">
-        <v>69.21673894162333</v>
+        <v>65.99557113041639</v>
       </c>
       <c r="EH34" t="n">
-        <v>0.002474298171313771</v>
+        <v>0.002359150740863949</v>
       </c>
       <c r="EI34" t="n">
-        <v>76.02433311589967</v>
+        <v>72.48635749835513</v>
       </c>
       <c r="EJ34" t="n">
-        <v>0.006935448495470461</v>
+        <v>0.006612690680070731</v>
       </c>
       <c r="EK34" t="n">
         <v>0</v>
       </c>
       <c r="EL34" t="n">
-        <v>0.8419255409158581</v>
+        <v>0.80274450619363</v>
       </c>
       <c r="EM34" t="n">
-        <v>0.0134228603257251</v>
+        <v>0.01279819516124776</v>
       </c>
       <c r="EN34" t="n">
-        <v>0.01387089699094117</v>
+        <v>0.01322538136014166</v>
       </c>
       <c r="EO34" t="n">
-        <v>0.09586487382025499</v>
+        <v>0.0914035708103241</v>
       </c>
       <c r="EP34" t="n">
-        <v>8.257238567830383</v>
+        <v>7.872968064902124</v>
       </c>
       <c r="EQ34" t="n">
-        <v>0.2520264709418379</v>
+        <v>0.2402978115426339</v>
       </c>
       <c r="ER34" t="n">
-        <v>0.05332873234749291</v>
+        <v>0.05084695122519476</v>
       </c>
       <c r="ES34" t="n">
-        <v>6.475151174335361</v>
+        <v>6.17381440443843</v>
       </c>
       <c r="ET34" t="n">
-        <v>0.1326625036779142</v>
+        <v>0.126488734252547</v>
       </c>
       <c r="EU34" t="n">
         <v>0</v>
@@ -19169,28 +19169,28 @@
       <c r="FB34" t="inlineStr"/>
       <c r="FC34" t="inlineStr"/>
       <c r="FD34" t="n">
-        <v>0.01633883006430314</v>
+        <v>0.01557846321835421</v>
       </c>
       <c r="FE34" t="n">
-        <v>0.02114788967649126</v>
+        <v>0.02016372164802749</v>
       </c>
       <c r="FF34" t="n">
-        <v>0.02145505812262826</v>
+        <v>0.02045659527001582</v>
       </c>
       <c r="FG34" t="n">
-        <v>0.0002906302885446408</v>
+        <v>0.0002771051074289666</v>
       </c>
       <c r="FH34" t="n">
-        <v>0.005221269542288433</v>
+        <v>0.004978285176939423</v>
       </c>
       <c r="FI34" t="n">
-        <v>0.01092733304764227</v>
+        <v>0.01041880326115391</v>
       </c>
       <c r="FJ34" t="n">
-        <v>0.004848911764890083</v>
+        <v>0.004623255966375513</v>
       </c>
       <c r="FK34" t="n">
-        <v>0.0001620004712502158</v>
+        <v>0.0001544613887772369</v>
       </c>
       <c r="FL34" t="n">
         <v>0</v>
@@ -19205,34 +19205,34 @@
         <v>0</v>
       </c>
       <c r="FP34" t="n">
-        <v>278.7443272965377</v>
+        <v>265.772288041678</v>
       </c>
       <c r="FQ34" t="n">
-        <v>0.03341188669458207</v>
+        <v>0.03185698399946534</v>
       </c>
       <c r="FR34" t="n">
-        <v>6.802799938503795</v>
+        <v>6.486215243485586</v>
       </c>
       <c r="FS34" t="n">
-        <v>6.298711945727663</v>
+        <v>6.005586200685641</v>
       </c>
       <c r="FT34" t="n">
-        <v>0.005099252217129193</v>
+        <v>0.004861946222160328</v>
       </c>
       <c r="FU34" t="n">
-        <v>0.002106671551580832</v>
+        <v>0.002008632512260287</v>
       </c>
       <c r="FV34" t="n">
-        <v>278.7443272965377</v>
+        <v>265.772288041678</v>
       </c>
       <c r="FW34" t="n">
-        <v>3.689141033329684e-07</v>
+        <v>3.517457962489164e-07</v>
       </c>
       <c r="FX34" t="n">
-        <v>3.643992016944374e-07</v>
+        <v>3.474410063831506e-07</v>
       </c>
       <c r="FY34" t="n">
-        <v>3.734299568132704e-07</v>
+        <v>3.560514935761004e-07</v>
       </c>
       <c r="FZ34" t="inlineStr">
         <is>
@@ -19571,31 +19571,31 @@
         </is>
       </c>
       <c r="CZ35" t="n">
-        <v>0.006435947568764484</v>
+        <v>0.006136435233163064</v>
       </c>
       <c r="DA35" t="n">
-        <v>0.01064774217943803</v>
+        <v>0.01015222382802648</v>
       </c>
       <c r="DB35" t="n">
-        <v>0.01128214602148505</v>
+        <v>0.01075710415789199</v>
       </c>
       <c r="DC35" t="n">
-        <v>1.472682139334392e-05</v>
+        <v>1.404147325705511e-05</v>
       </c>
       <c r="DD35" t="n">
-        <v>0.01624254301821817</v>
+        <v>0.0154866571220783</v>
       </c>
       <c r="DE35" t="n">
-        <v>0.02847300108241831</v>
+        <v>0.02714794133563512</v>
       </c>
       <c r="DF35" t="n">
-        <v>2.716202107727562e-06</v>
+        <v>2.589797094548286e-06</v>
       </c>
       <c r="DG35" t="n">
-        <v>0.02854462864111884</v>
+        <v>0.02721623553321506</v>
       </c>
       <c r="DH35" t="n">
-        <v>0.01187714892836912</v>
+        <v>0.01132441717009834</v>
       </c>
       <c r="DI35" t="n">
         <v>0</v>
@@ -19609,97 +19609,97 @@
       <c r="DL35" t="inlineStr"/>
       <c r="DM35" t="inlineStr"/>
       <c r="DN35" t="n">
-        <v>0.006435947568764484</v>
+        <v>0.006136435233163064</v>
       </c>
       <c r="DO35" t="n">
-        <v>0.01064774217943803</v>
+        <v>0.01015222382802648</v>
       </c>
       <c r="DP35" t="n">
-        <v>0.006522532204919473</v>
+        <v>0.006218990444540284</v>
       </c>
       <c r="DQ35" t="n">
-        <v>0.01114679390918582</v>
+        <v>0.01062805098243931</v>
       </c>
       <c r="DR35" t="n">
-        <v>0.01171766554538089</v>
+        <v>0.01117235573081273</v>
       </c>
       <c r="DS35" t="n">
-        <v>0.02052081621603466</v>
+        <v>0.01956583056277334</v>
       </c>
       <c r="DT35" t="n">
-        <v>0.01622059036307929</v>
+        <v>0.01546572608668371</v>
       </c>
       <c r="DU35" t="n">
-        <v>0.02854462864111884</v>
+        <v>0.02721623553321507</v>
       </c>
       <c r="DV35" t="n">
-        <v>0.002394959997768867</v>
+        <v>0.002283504760641688</v>
       </c>
       <c r="DW35" t="n">
-        <v>0.02897175233214664</v>
+        <v>0.02762348199359057</v>
       </c>
       <c r="DX35" t="n">
-        <v>8.392091765596962</v>
+        <v>8.001545544012693</v>
       </c>
       <c r="DY35" t="n">
-        <v>0.002394959997768867</v>
+        <v>0.002283504760641688</v>
       </c>
       <c r="DZ35" t="n">
-        <v>12.53705105258549</v>
+        <v>11.95360915810232</v>
       </c>
       <c r="EA35" t="n">
-        <v>0.02193412203468964</v>
+        <v>0.02091336478802399</v>
       </c>
       <c r="EB35" t="n">
-        <v>4.402603051433692</v>
+        <v>4.197717304840514</v>
       </c>
       <c r="EC35" t="n">
-        <v>0.05993873314881612</v>
+        <v>0.0571493397041708</v>
       </c>
       <c r="ED35" t="n">
-        <v>0.04386824406937911</v>
+        <v>0.04182672957604781</v>
       </c>
       <c r="EE35" t="n">
-        <v>0.01423306168665726</v>
+        <v>0.01357069184865537</v>
       </c>
       <c r="EF35" t="n">
-        <v>0.001129525032956536</v>
+        <v>0.001076959862540452</v>
       </c>
       <c r="EG35" t="n">
-        <v>15.71531100505794</v>
+        <v>14.9839611216823</v>
       </c>
       <c r="EH35" t="n">
-        <v>0.01423306168676023</v>
+        <v>0.01357069184875303</v>
       </c>
       <c r="EI35" t="n">
-        <v>25.19342739523132</v>
+        <v>24.02099051622806</v>
       </c>
       <c r="EJ35" t="n">
-        <v>0.008627218785594037</v>
+        <v>0.008225730361300703</v>
       </c>
       <c r="EK35" t="n">
         <v>0</v>
       </c>
       <c r="EL35" t="n">
-        <v>0.6716759397494474</v>
+        <v>0.6404178806474745</v>
       </c>
       <c r="EM35" t="n">
-        <v>0.05303800523909073</v>
+        <v>0.05056975380368477</v>
       </c>
       <c r="EN35" t="n">
-        <v>0.0172544375711881</v>
+        <v>0.01645146072260143</v>
       </c>
       <c r="EO35" t="inlineStr"/>
       <c r="EP35" t="inlineStr"/>
       <c r="EQ35" t="inlineStr"/>
       <c r="ER35" t="n">
-        <v>0.04803598284116244</v>
+        <v>0.04580051257663533</v>
       </c>
       <c r="ES35" t="n">
-        <v>5.450661487686125</v>
+        <v>5.197001815150445</v>
       </c>
       <c r="ET35" t="n">
-        <v>0.03087179621122499</v>
+        <v>0.02943510275021679</v>
       </c>
       <c r="EU35" t="inlineStr"/>
       <c r="EV35" t="inlineStr"/>
@@ -19711,28 +19711,28 @@
       <c r="FB35" t="inlineStr"/>
       <c r="FC35" t="inlineStr"/>
       <c r="FD35" t="n">
-        <v>0.04423884513694672</v>
+        <v>0.04218008382950799</v>
       </c>
       <c r="FE35" t="n">
-        <v>0.09004772594196496</v>
+        <v>0.08585713793230346</v>
       </c>
       <c r="FF35" t="n">
-        <v>0.0568721599923593</v>
+        <v>0.0542254769223045</v>
       </c>
       <c r="FG35" t="n">
-        <v>0.0003308651139895272</v>
+        <v>0.0003154675082754932</v>
       </c>
       <c r="FH35" t="n">
-        <v>0.02039878347673135</v>
+        <v>0.01944947691118454</v>
       </c>
       <c r="FI35" t="n">
-        <v>0.02363730315891303</v>
+        <v>0.02253728427268023</v>
       </c>
       <c r="FJ35" t="n">
-        <v>0.02075300298690273</v>
+        <v>0.01978721196251378</v>
       </c>
       <c r="FK35" t="n">
-        <v>8.539841672179563e-05</v>
+        <v>8.142419552503738e-05</v>
       </c>
       <c r="FL35" t="n">
         <v>0</v>
@@ -19747,34 +19747,34 @@
         <v>0</v>
       </c>
       <c r="FP35" t="n">
-        <v>425.3741882155055</v>
+        <v>405.5783748941982</v>
       </c>
       <c r="FQ35" t="n">
-        <v>0.06682377338940046</v>
+        <v>0.06371396799902426</v>
       </c>
       <c r="FR35" t="n">
-        <v>5.283080935150824</v>
+        <v>5.037220027622929</v>
       </c>
       <c r="FS35" t="n">
-        <v>0.4114359576865466</v>
+        <v>0.3922887935245519</v>
       </c>
       <c r="FT35" t="n">
-        <v>0.005259913319722202</v>
+        <v>0.005015130573029707</v>
       </c>
       <c r="FU35" t="n">
-        <v>0.002126249051058417</v>
+        <v>0.002027298925603145</v>
       </c>
       <c r="FV35" t="n">
-        <v>425.3741882155055</v>
+        <v>405.5783748941982</v>
       </c>
       <c r="FW35" t="n">
-        <v>5.629766128099949e-07</v>
+        <v>5.367771389076341e-07</v>
       </c>
       <c r="FX35" t="n">
-        <v>5.901983981669165e-07</v>
+        <v>5.627320928767214e-07</v>
       </c>
       <c r="FY35" t="n">
-        <v>5.357567290249659e-07</v>
+        <v>5.108239979813194e-07</v>
       </c>
       <c r="FZ35" t="inlineStr">
         <is>
@@ -20093,31 +20093,31 @@
         </is>
       </c>
       <c r="CZ36" t="n">
-        <v>0.001063819552581459</v>
+        <v>0.001014312145094404</v>
       </c>
       <c r="DA36" t="n">
-        <v>0.0001207662537148992</v>
+        <v>0.0001151461049604975</v>
       </c>
       <c r="DB36" t="n">
-        <v>0.0001441863020873739</v>
+        <v>0.0001374762449219746</v>
       </c>
       <c r="DC36" t="n">
-        <v>1.865181337646678e-06</v>
+        <v>1.778380627605027e-06</v>
       </c>
       <c r="DD36" t="n">
-        <v>0.002684784899468948</v>
+        <v>0.002559841961813934</v>
       </c>
       <c r="DE36" t="n">
-        <v>0.0003638861549490217</v>
+        <v>0.0003469518354883165</v>
       </c>
       <c r="DF36" t="n">
-        <v>2.411020101903809e-06</v>
+        <v>2.298817469084363e-06</v>
       </c>
       <c r="DG36" t="n">
-        <v>0.0003651317630034682</v>
+        <v>0.000348139476169094</v>
       </c>
       <c r="DH36" t="n">
-        <v>0.01084435336938104</v>
+        <v>0.01033968524226356</v>
       </c>
       <c r="DI36" t="n">
         <v>0</v>
@@ -20131,85 +20131,85 @@
       <c r="DL36" t="inlineStr"/>
       <c r="DM36" t="inlineStr"/>
       <c r="DN36" t="n">
-        <v>0.001063819552581459</v>
+        <v>0.001014312145094404</v>
       </c>
       <c r="DO36" t="n">
-        <v>0.0001207662537148992</v>
+        <v>0.0001151461049604975</v>
       </c>
       <c r="DP36" t="n">
-        <v>0.001075060579604319</v>
+        <v>0.001025030043825404</v>
       </c>
       <c r="DQ36" t="n">
-        <v>0.0001353053089271395</v>
+        <v>0.0001290085501883448</v>
       </c>
       <c r="DR36" t="n">
-        <v>0.001952375146233779</v>
+        <v>0.001861516662106801</v>
       </c>
       <c r="DS36" t="n">
-        <v>0.0002596563784014416</v>
+        <v>0.0002475726428647713</v>
       </c>
       <c r="DT36" t="n">
-        <v>0.002673323868098246</v>
+        <v>0.002548914297169838</v>
       </c>
       <c r="DU36" t="n">
-        <v>0.0003651317630034683</v>
+        <v>0.0003481394761690951</v>
       </c>
       <c r="DV36" t="n">
-        <v>0.005875469164833302</v>
+        <v>0.005602040042932474</v>
       </c>
       <c r="DW36" t="n">
-        <v>0.000329064610910153</v>
+        <v>0.0003137507959474874</v>
       </c>
       <c r="DX36" t="n">
-        <v>3.506831981157319</v>
+        <v>3.343633100803501</v>
       </c>
       <c r="DY36" t="n">
-        <v>0.005875469164833302</v>
+        <v>0.005602040042932474</v>
       </c>
       <c r="DZ36" t="n">
-        <v>8.607481751254587</v>
+        <v>8.206911837435381</v>
       </c>
       <c r="EA36" t="n">
-        <v>0.01527907141721977</v>
+        <v>0.01456802299473068</v>
       </c>
       <c r="EB36" t="n">
-        <v>0.1040658108558783</v>
+        <v>0.09922285747058783</v>
       </c>
       <c r="EC36" t="n">
-        <v>0.0867505685528956</v>
+        <v>0.08271342171097108</v>
       </c>
       <c r="ED36" t="n">
-        <v>0.03055814283443959</v>
+        <v>0.02913604598946133</v>
       </c>
       <c r="EE36" t="n">
-        <v>0.00747069949733105</v>
+        <v>0.007123032486102711</v>
       </c>
       <c r="EF36" t="n">
-        <v>0.0002081164502214413</v>
+        <v>0.0001984312494927369</v>
       </c>
       <c r="EG36" t="n">
-        <v>3.802732066863794</v>
+        <v>3.625762762679198</v>
       </c>
       <c r="EH36" t="n">
-        <v>0.00747069949733105</v>
+        <v>0.007123032486102711</v>
       </c>
       <c r="EI36" t="n">
-        <v>9.860126036153739</v>
+        <v>9.401261300719026</v>
       </c>
       <c r="EJ36" t="n">
-        <v>0.00969101307233452</v>
+        <v>0.009240018416360966</v>
       </c>
       <c r="EK36" t="n">
         <v>0</v>
       </c>
       <c r="EL36" t="n">
-        <v>0.09115297354844679</v>
+        <v>0.08691095017693695</v>
       </c>
       <c r="EM36" t="n">
-        <v>0.01816114659518298</v>
+        <v>0.01731597385631194</v>
       </c>
       <c r="EN36" t="n">
-        <v>0.01938202614466904</v>
+        <v>0.01848003683272193</v>
       </c>
       <c r="EO36" t="inlineStr"/>
       <c r="EP36" t="inlineStr"/>
@@ -20227,28 +20227,28 @@
       <c r="FB36" t="inlineStr"/>
       <c r="FC36" t="inlineStr"/>
       <c r="FD36" t="n">
-        <v>0.07293451192471589</v>
+        <v>0.06954032858510313</v>
       </c>
       <c r="FE36" t="n">
-        <v>0.05482058709123093</v>
+        <v>0.05226937891196855</v>
       </c>
       <c r="FF36" t="n">
-        <v>0.08494464893594096</v>
+        <v>0.08099154491702011</v>
       </c>
       <c r="FG36" t="n">
-        <v>0.0005502957066553749</v>
+        <v>0.0005246863693183666</v>
       </c>
       <c r="FH36" t="n">
-        <v>0.01263988208993096</v>
+        <v>0.01205165470522441</v>
       </c>
       <c r="FI36" t="n">
-        <v>0.009799169712614339</v>
+        <v>0.009343141726646262</v>
       </c>
       <c r="FJ36" t="n">
-        <v>0.01392693226356921</v>
+        <v>0.01327880889627069</v>
       </c>
       <c r="FK36" t="n">
-        <v>8.152312175217645e-06</v>
+        <v>7.772924674921477e-06</v>
       </c>
       <c r="FL36" t="n">
         <v>0</v>
@@ -20263,7 +20263,7 @@
         <v>0</v>
       </c>
       <c r="FP36" t="n">
-        <v>232.1935973851712</v>
+        <v>221.3879085691137</v>
       </c>
       <c r="FQ36" t="inlineStr"/>
       <c r="FR36" t="inlineStr"/>
@@ -20271,16 +20271,16 @@
       <c r="FT36" t="inlineStr"/>
       <c r="FU36" t="inlineStr"/>
       <c r="FV36" t="n">
-        <v>232.1935973851712</v>
+        <v>221.3879085691137</v>
       </c>
       <c r="FW36" t="n">
-        <v>3.073048825935474e-07</v>
+        <v>2.930037090473629e-07</v>
       </c>
       <c r="FX36" t="n">
-        <v>3.307352032162468e-07</v>
+        <v>3.153436431989668e-07</v>
       </c>
       <c r="FY36" t="n">
-        <v>2.838750089882686e-07</v>
+        <v>2.706642011849274e-07</v>
       </c>
       <c r="FZ36" t="inlineStr">
         <is>
@@ -20301,7 +20301,7 @@
         <v>0.1168176862369729</v>
       </c>
       <c r="D37" t="n">
-        <v>0.01060195418955971</v>
+        <v>0.0106019541895597</v>
       </c>
       <c r="E37" t="n">
         <v>0.009638007229164932</v>
@@ -20349,7 +20349,7 @@
         <v>0.1168176862369729</v>
       </c>
       <c r="T37" t="n">
-        <v>0.01060195418955971</v>
+        <v>0.0106019541895597</v>
       </c>
       <c r="U37" t="n">
         <v>0.1198878083644862</v>
@@ -20599,31 +20599,31 @@
         </is>
       </c>
       <c r="CZ37" t="n">
-        <v>0.01643148324424374</v>
+        <v>0.0156668045592022</v>
       </c>
       <c r="DA37" t="n">
-        <v>0.006269397364245392</v>
+        <v>0.005977635843922903</v>
       </c>
       <c r="DB37" t="n">
-        <v>0.006717733537387882</v>
+        <v>0.006405107612419802</v>
       </c>
       <c r="DC37" t="n">
-        <v>2.105898275511169e-05</v>
+        <v>2.007895222456721e-05</v>
       </c>
       <c r="DD37" t="n">
-        <v>0.04146849715541996</v>
+        <v>0.03953866066992996</v>
       </c>
       <c r="DE37" t="n">
-        <v>0.0169536924905201</v>
+        <v>0.01616471153928484</v>
       </c>
       <c r="DF37" t="n">
-        <v>2.924987720058382e-06</v>
+        <v>2.788866365078442e-06</v>
       </c>
       <c r="DG37" t="n">
-        <v>0.01699734081827775</v>
+        <v>0.0162063285868849</v>
       </c>
       <c r="DH37" t="n">
-        <v>0.01632176461048252</v>
+        <v>0.01556219194656709</v>
       </c>
       <c r="DI37" t="n">
         <v>0</v>
@@ -20637,85 +20637,85 @@
       <c r="DL37" t="inlineStr"/>
       <c r="DM37" t="inlineStr"/>
       <c r="DN37" t="n">
-        <v>0.01643148324424374</v>
+        <v>0.0156668045592022</v>
       </c>
       <c r="DO37" t="n">
-        <v>0.006269397364245392</v>
+        <v>0.005977635843922903</v>
       </c>
       <c r="DP37" t="n">
-        <v>0.01656602257727613</v>
+        <v>0.01579508278003064</v>
       </c>
       <c r="DQ37" t="n">
-        <v>0.006540001389646825</v>
+        <v>0.006235646658642434</v>
       </c>
       <c r="DR37" t="n">
-        <v>0.03036750923293743</v>
+        <v>0.02895428398217595</v>
       </c>
       <c r="DS37" t="n">
-        <v>0.01261096553284711</v>
+        <v>0.01202408384983533</v>
       </c>
       <c r="DT37" t="n">
-        <v>0.04156719552928631</v>
+        <v>0.03963276587703544</v>
       </c>
       <c r="DU37" t="n">
-        <v>0.01699734081827775</v>
+        <v>0.0162063285868849</v>
       </c>
       <c r="DV37" t="n">
-        <v>0.03749896731643135</v>
+        <v>0.03575386247148448</v>
       </c>
       <c r="DW37" t="n">
-        <v>0.0156794394419207</v>
+        <v>0.01494975892821317</v>
       </c>
       <c r="DX37" t="n">
-        <v>50.32846072112241</v>
+        <v>47.98630447190646</v>
       </c>
       <c r="DY37" t="n">
-        <v>0.03749896731643135</v>
+        <v>0.03575386247148448</v>
       </c>
       <c r="DZ37" t="n">
-        <v>79.44766123779584</v>
+        <v>75.75037279329551</v>
       </c>
       <c r="EA37" t="n">
-        <v>0.0532038269095138</v>
+        <v>0.05072785856291934</v>
       </c>
       <c r="EB37" t="n">
-        <v>0.319400487057519</v>
+        <v>0.3045364153961654</v>
       </c>
       <c r="EC37" t="n">
-        <v>0.2624068981485784</v>
+        <v>0.250195160544648</v>
       </c>
       <c r="ED37" t="n">
-        <v>0.1064076538190271</v>
+        <v>0.1014557171258382</v>
       </c>
       <c r="EE37" t="n">
-        <v>0.005210632675607863</v>
+        <v>0.004968143322405316</v>
       </c>
       <c r="EF37" t="n">
-        <v>0.00670485483880123</v>
+        <v>0.00639282825511926</v>
       </c>
       <c r="EG37" t="n">
-        <v>92.7745973160421</v>
+        <v>88.45710777317068</v>
       </c>
       <c r="EH37" t="n">
-        <v>0.005210632675607863</v>
+        <v>0.004968143322405316</v>
       </c>
       <c r="EI37" t="n">
-        <v>120.7944442177325</v>
+        <v>115.1729835503215</v>
       </c>
       <c r="EJ37" t="n">
-        <v>0.01446855800552933</v>
+        <v>0.01379522877860202</v>
       </c>
       <c r="EK37" t="n">
         <v>0</v>
       </c>
       <c r="EL37" t="n">
-        <v>0.3101793463003828</v>
+        <v>0.2957444026540684</v>
       </c>
       <c r="EM37" t="n">
-        <v>0.1123492063391894</v>
+        <v>0.1071207651758508</v>
       </c>
       <c r="EN37" t="n">
-        <v>0.02893711601105849</v>
+        <v>0.02759045755720392</v>
       </c>
       <c r="EO37" t="inlineStr"/>
       <c r="EP37" t="inlineStr"/>
@@ -20733,28 +20733,28 @@
       <c r="FB37" t="inlineStr"/>
       <c r="FC37" t="inlineStr"/>
       <c r="FD37" t="n">
-        <v>0.06168941019181493</v>
+        <v>0.05881854477052132</v>
       </c>
       <c r="FE37" t="n">
-        <v>0.06356147722886593</v>
+        <v>0.06060349065490931</v>
       </c>
       <c r="FF37" t="n">
-        <v>0.05158293940848747</v>
+        <v>0.04918240296931495</v>
       </c>
       <c r="FG37" t="n">
-        <v>0.008858838941151177</v>
+        <v>0.008446571514539683</v>
       </c>
       <c r="FH37" t="n">
-        <v>0.01381915393590247</v>
+        <v>0.01317604629290899</v>
       </c>
       <c r="FI37" t="n">
-        <v>0.01874347249281141</v>
+        <v>0.01787119981444951</v>
       </c>
       <c r="FJ37" t="n">
-        <v>0.01480157818862128</v>
+        <v>0.01411275106464393</v>
       </c>
       <c r="FK37" t="n">
-        <v>0.005931306330024397</v>
+        <v>0.005655278691033835</v>
       </c>
       <c r="FL37" t="n">
         <v>0</v>
@@ -20769,7 +20769,7 @@
         <v>0</v>
       </c>
       <c r="FP37" t="n">
-        <v>234.7884153871307</v>
+        <v>223.8619704598829</v>
       </c>
       <c r="FQ37" t="inlineStr"/>
       <c r="FR37" t="inlineStr"/>
@@ -20777,16 +20777,16 @@
       <c r="FT37" t="inlineStr"/>
       <c r="FU37" t="inlineStr"/>
       <c r="FV37" t="n">
-        <v>234.7884153871307</v>
+        <v>223.8619704598829</v>
       </c>
       <c r="FW37" t="n">
-        <v>3.107390868456532e-07</v>
+        <v>2.962780944080793e-07</v>
       </c>
       <c r="FX37" t="n">
-        <v>3.383773000242606e-07</v>
+        <v>3.226300966598488e-07</v>
       </c>
       <c r="FY37" t="n">
-        <v>2.831013022361964e-07</v>
+        <v>2.699265006804926e-07</v>
       </c>
       <c r="FZ37" t="inlineStr">
         <is>

</xml_diff>